<commit_message>
Adapt some details in figures
</commit_message>
<xml_diff>
--- a/vein_data/vein_general.xlsx
+++ b/vein_data/vein_general.xlsx
@@ -97,13 +97,13 @@
     <t>sub_leaf_1</t>
   </si>
   <si>
-    <t>-7.269803141656649</t>
-  </si>
-  <si>
-    <t>-0.43161909959456324</t>
-  </si>
-  <si>
-    <t>52.90567091448799</t>
+    <t>-6.911871570822404</t>
+  </si>
+  <si>
+    <t>-0.21521026486142603</t>
+  </si>
+  <si>
+    <t>52.98480893488265</t>
   </si>
   <si>
     <t>27.41348121881259</t>
@@ -127,28 +127,28 @@
     <t>4</t>
   </si>
   <si>
-    <t>-75.8524720069338</t>
-  </si>
-  <si>
-    <t>-41.56697009789943</t>
-  </si>
-  <si>
-    <t>40.7037318987103</t>
-  </si>
-  <si>
-    <t>47.636497639496326</t>
+    <t>-75.28451095800045</t>
+  </si>
+  <si>
+    <t>-41.70211347736648</t>
+  </si>
+  <si>
+    <t>41.27169294764363</t>
+  </si>
+  <si>
+    <t>48.06744520443369</t>
   </si>
   <si>
     <t>sub_leaf_2</t>
   </si>
   <si>
-    <t>-0.13785200771254935</t>
-  </si>
-  <si>
-    <t>1.4286945420264594</t>
-  </si>
-  <si>
-    <t>42.51768009191312</t>
+    <t>-0.3543272665957655</t>
+  </si>
+  <si>
+    <t>1.1170705284749474</t>
+  </si>
+  <si>
+    <t>42.304583654301275</t>
   </si>
   <si>
     <t>0.1650105616827134</t>
@@ -169,28 +169,28 @@
     <t>0.38962323077198296</t>
   </si>
   <si>
-    <t>-45.85565184946913</t>
-  </si>
-  <si>
-    <t>42.18731249400858</t>
-  </si>
-  <si>
-    <t>42.44685473456602</t>
-  </si>
-  <si>
-    <t>-39.32992340995566</t>
+    <t>-45.85820751037421</t>
+  </si>
+  <si>
+    <t>41.56662012781063</t>
+  </si>
+  <si>
+    <t>42.20675738704125</t>
+  </si>
+  <si>
+    <t>-39.332479070860735</t>
   </si>
   <si>
     <t>sub_leaf_3</t>
   </si>
   <si>
-    <t>33.84728719916341</t>
-  </si>
-  <si>
-    <t>51.411795564997774</t>
-  </si>
-  <si>
-    <t>44.91510478700864</t>
+    <t>33.92451846423617</t>
+  </si>
+  <si>
+    <t>51.52438930839696</t>
+  </si>
+  <si>
+    <t>44.88061590021839</t>
   </si>
   <si>
     <t>0.15044135295302438</t>
@@ -211,28 +211,28 @@
     <t>163.26074768674525</t>
   </si>
   <si>
-    <t>74.23875232704243</t>
-  </si>
-  <si>
-    <t>-41.67319466038433</t>
-  </si>
-  <si>
-    <t>59.08085705810068</t>
-  </si>
-  <si>
-    <t>43.742734071894866</t>
+    <t>74.2225939885502</t>
+  </si>
+  <si>
+    <t>-41.57329874839941</t>
+  </si>
+  <si>
+    <t>59.064698719608465</t>
+  </si>
+  <si>
+    <t>43.98407989718545</t>
   </si>
   <si>
     <t>sub_leaf_4</t>
   </si>
   <si>
-    <t>21.927697114325888</t>
-  </si>
-  <si>
-    <t>46.655580019932344</t>
-  </si>
-  <si>
-    <t>48.13994149196195</t>
+    <t>22.181912640697156</t>
+  </si>
+  <si>
+    <t>46.96518492533878</t>
+  </si>
+  <si>
+    <t>48.05680886903047</t>
   </si>
   <si>
     <t>2.85908802149332</t>
@@ -253,28 +253,28 @@
     <t>38.81331819256618</t>
   </si>
   <si>
-    <t>55.600274273070184</t>
-  </si>
-  <si>
-    <t>-61.20064585563132</t>
-  </si>
-  <si>
-    <t>45.49032812251029</t>
-  </si>
-  <si>
-    <t>47.82083191735439</t>
+    <t>55.60490802532658</t>
+  </si>
+  <si>
+    <t>-60.80762731321552</t>
+  </si>
+  <si>
+    <t>45.37679231239601</t>
+  </si>
+  <si>
+    <t>48.55357753828155</t>
   </si>
   <si>
     <t>sub_leaf_5</t>
   </si>
   <si>
-    <t>-7.1256225321581095</t>
-  </si>
-  <si>
-    <t>-4.848452993767175</t>
-  </si>
-  <si>
-    <t>46.6713117996562</t>
+    <t>-7.045877421782528</t>
+  </si>
+  <si>
+    <t>-4.893257402698325</t>
+  </si>
+  <si>
+    <t>46.52843976698257</t>
   </si>
   <si>
     <t>0.39428273522074164</t>
@@ -295,28 +295,28 @@
     <t>11.52428125156565</t>
   </si>
   <si>
-    <t>-63.82957183090801</t>
-  </si>
-  <si>
-    <t>45.02398768980992</t>
-  </si>
-  <si>
-    <t>-42.04761068457632</t>
-  </si>
-  <si>
-    <t>32.35070469704197</t>
+    <t>-63.420982772657304</t>
+  </si>
+  <si>
+    <t>45.02398789092384</t>
+  </si>
+  <si>
+    <t>-42.0476104834624</t>
+  </si>
+  <si>
+    <t>32.26109567806575</t>
   </si>
   <si>
     <t>sub_leaf_6</t>
   </si>
   <si>
-    <t>-35.564007540903695</t>
-  </si>
-  <si>
-    <t>-63.883294897021365</t>
-  </si>
-  <si>
-    <t>50.75169518222968</t>
+    <t>-35.69223966761786</t>
+  </si>
+  <si>
+    <t>-64.12503882579095</t>
+  </si>
+  <si>
+    <t>50.72933203675473</t>
   </si>
   <si>
     <t>154.59292641032692</t>
@@ -340,22 +340,22 @@
     <t>3</t>
   </si>
   <si>
-    <t>-78.51929464750184</t>
-  </si>
-  <si>
-    <t>35.71056692181213</t>
+    <t>-78.5186279093085</t>
+  </si>
+  <si>
+    <t>35.56694773224588</t>
   </si>
   <si>
     <t>sub_leaf_7</t>
   </si>
   <si>
-    <t>6.064262232990359</t>
-  </si>
-  <si>
-    <t>39.48392088041281</t>
-  </si>
-  <si>
-    <t>44.01177197881365</t>
+    <t>6.070738168030725</t>
+  </si>
+  <si>
+    <t>39.363418170605705</t>
+  </si>
+  <si>
+    <t>44.02958802570318</t>
   </si>
   <si>
     <t>0.0724181127538227</t>
@@ -379,28 +379,28 @@
     <t>5</t>
   </si>
   <si>
-    <t>-49.9865103968199</t>
+    <t>-50.014966639368545</t>
   </si>
   <si>
     <t>-45.554068369370086</t>
   </si>
   <si>
-    <t>44.87356196794846</t>
-  </si>
-  <si>
-    <t>41.5044070827805</t>
+    <t>44.842795260311505</t>
+  </si>
+  <si>
+    <t>41.71651241797505</t>
   </si>
   <si>
     <t>sub_leaf_8</t>
   </si>
   <si>
-    <t>-13.344098369914013</t>
-  </si>
-  <si>
-    <t>-12.224789372155314</t>
-  </si>
-  <si>
-    <t>47.94792506179109</t>
+    <t>-13.351267345975979</t>
+  </si>
+  <si>
+    <t>-12.371830583187212</t>
+  </si>
+  <si>
+    <t>48.1214049460452</t>
   </si>
   <si>
     <t>0.28126467975090946</t>
@@ -424,34 +424,34 @@
     <t>6</t>
   </si>
   <si>
-    <t>30.58799108325697</t>
-  </si>
-  <si>
-    <t>-71.621461170182</t>
-  </si>
-  <si>
-    <t>-52.46264048770476</t>
-  </si>
-  <si>
-    <t>28.013061743394132</t>
-  </si>
-  <si>
-    <t>-58.05385287867633</t>
-  </si>
-  <si>
-    <t>43.47231149042792</t>
+    <t>30.720433098962136</t>
+  </si>
+  <si>
+    <t>-71.62470029295248</t>
+  </si>
+  <si>
+    <t>-52.75348378699806</t>
+  </si>
+  <si>
+    <t>28.009822620623638</t>
+  </si>
+  <si>
+    <t>-58.306700010311275</t>
+  </si>
+  <si>
+    <t>43.84702429482017</t>
   </si>
   <si>
     <t>sub_leaf_9</t>
   </si>
   <si>
-    <t>-24.24420826990227</t>
-  </si>
-  <si>
-    <t>-47.136113688328564</t>
-  </si>
-  <si>
-    <t>51.50806254849579</t>
+    <t>-24.21582632878154</t>
+  </si>
+  <si>
+    <t>-47.6048969763473</t>
+  </si>
+  <si>
+    <t>51.567206126551696</t>
   </si>
   <si>
     <t>0.7133938885508732</t>
@@ -472,28 +472,28 @@
     <t>149.0391599568673</t>
   </si>
   <si>
-    <t>-92.16107565953361</t>
-  </si>
-  <si>
-    <t>-53.79616980310808</t>
-  </si>
-  <si>
-    <t>38.38470048171806</t>
-  </si>
-  <si>
-    <t>33.48761731974084</t>
+    <t>-92.16758154716233</t>
+  </si>
+  <si>
+    <t>-53.43252148827322</t>
+  </si>
+  <si>
+    <t>38.378194594089344</t>
+  </si>
+  <si>
+    <t>33.74767377378584</t>
   </si>
   <si>
     <t>sub_leaf_10</t>
   </si>
   <si>
-    <t>0.46921153871572585</t>
-  </si>
-  <si>
-    <t>1.0200355672375991</t>
-  </si>
-  <si>
-    <t>39.38441442238943</t>
+    <t>0.5436438980255804</t>
+  </si>
+  <si>
+    <t>1.1107880255880183</t>
+  </si>
+  <si>
+    <t>39.31185151147227</t>
   </si>
   <si>
     <t>12.923498989878858</t>
@@ -514,16 +514,16 @@
     <t>16.76451972611114</t>
   </si>
   <si>
-    <t>-41.49561835042494</t>
-  </si>
-  <si>
-    <t>38.25627467841626</t>
-  </si>
-  <si>
-    <t>41.332393370812646</t>
-  </si>
-  <si>
-    <t>-36.21620354394106</t>
+    <t>-41.49590915749956</t>
+  </si>
+  <si>
+    <t>38.12753195734236</t>
+  </si>
+  <si>
+    <t>41.448908698425846</t>
+  </si>
+  <si>
+    <t>-35.90595590616633</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Colorize the numbers of sub veins in the colored_veins.jpg
</commit_message>
<xml_diff>
--- a/vein_data/vein_general.xlsx
+++ b/vein_data/vein_general.xlsx
@@ -97,13 +97,13 @@
     <t>sub_leaf_1</t>
   </si>
   <si>
-    <t>-6.911871570822404</t>
-  </si>
-  <si>
-    <t>-0.21521026486142603</t>
-  </si>
-  <si>
-    <t>52.98480893488265</t>
+    <t>-6.782253339837299</t>
+  </si>
+  <si>
+    <t>-0.20456564967241775</t>
+  </si>
+  <si>
+    <t>53.10851737952483</t>
   </si>
   <si>
     <t>27.41348121881259</t>
@@ -127,28 +127,28 @@
     <t>4</t>
   </si>
   <si>
-    <t>-75.28451095800045</t>
-  </si>
-  <si>
-    <t>-41.70211347736648</t>
-  </si>
-  <si>
-    <t>41.27169294764363</t>
-  </si>
-  <si>
-    <t>48.06744520443369</t>
+    <t>-75.27386634281146</t>
+  </si>
+  <si>
+    <t>-41.69146886217747</t>
+  </si>
+  <si>
+    <t>41.28233756283264</t>
+  </si>
+  <si>
+    <t>48.5539842828071</t>
   </si>
   <si>
     <t>sub_leaf_2</t>
   </si>
   <si>
-    <t>-0.3543272665957655</t>
-  </si>
-  <si>
-    <t>1.1170705284749474</t>
-  </si>
-  <si>
-    <t>42.304583654301275</t>
+    <t>-0.30890568620245773</t>
+  </si>
+  <si>
+    <t>1.34241802464701</t>
+  </si>
+  <si>
+    <t>42.580041408615855</t>
   </si>
   <si>
     <t>0.1650105616827134</t>
@@ -169,28 +169,28 @@
     <t>0.38962323077198296</t>
   </si>
   <si>
-    <t>-45.85820751037421</t>
-  </si>
-  <si>
-    <t>41.56662012781063</t>
-  </si>
-  <si>
-    <t>42.20675738704125</t>
-  </si>
-  <si>
-    <t>-39.332479070860735</t>
+    <t>-46.288270262894805</t>
+  </si>
+  <si>
+    <t>42.03259995738133</t>
+  </si>
+  <si>
+    <t>42.367811468790954</t>
+  </si>
+  <si>
+    <t>-39.34776390808731</t>
   </si>
   <si>
     <t>sub_leaf_3</t>
   </si>
   <si>
-    <t>33.92451846423617</t>
-  </si>
-  <si>
-    <t>51.52438930839696</t>
-  </si>
-  <si>
-    <t>44.88061590021839</t>
+    <t>33.92211654331513</t>
+  </si>
+  <si>
+    <t>51.48826472585644</t>
+  </si>
+  <si>
+    <t>44.875099521691986</t>
   </si>
   <si>
     <t>0.15044135295302438</t>
@@ -211,28 +211,28 @@
     <t>163.26074768674525</t>
   </si>
   <si>
-    <t>74.2225939885502</t>
-  </si>
-  <si>
-    <t>-41.57329874839941</t>
-  </si>
-  <si>
-    <t>59.064698719608465</t>
-  </si>
-  <si>
-    <t>43.98407989718545</t>
+    <t>74.2387529794948</t>
+  </si>
+  <si>
+    <t>-41.52681625794717</t>
+  </si>
+  <si>
+    <t>59.233794727365634</t>
+  </si>
+  <si>
+    <t>43.74273472434724</t>
   </si>
   <si>
     <t>sub_leaf_4</t>
   </si>
   <si>
-    <t>22.181912640697156</t>
-  </si>
-  <si>
-    <t>46.96518492533878</t>
-  </si>
-  <si>
-    <t>48.05680886903047</t>
+    <t>21.996248083321447</t>
+  </si>
+  <si>
+    <t>46.805060137145375</t>
+  </si>
+  <si>
+    <t>48.1850912717703</t>
   </si>
   <si>
     <t>2.85908802149332</t>
@@ -253,28 +253,28 @@
     <t>38.81331819256618</t>
   </si>
   <si>
-    <t>55.60490802532658</t>
-  </si>
-  <si>
-    <t>-60.80762731321552</t>
-  </si>
-  <si>
-    <t>45.37679231239601</t>
-  </si>
-  <si>
-    <t>48.55357753828155</t>
+    <t>55.59021296997648</t>
+  </si>
+  <si>
+    <t>-61.215340910981425</t>
+  </si>
+  <si>
+    <t>45.47563306716019</t>
+  </si>
+  <si>
+    <t>48.134487207130555</t>
   </si>
   <si>
     <t>sub_leaf_5</t>
   </si>
   <si>
-    <t>-7.045877421782528</t>
-  </si>
-  <si>
-    <t>-4.893257402698325</t>
-  </si>
-  <si>
-    <t>46.52843976698257</t>
+    <t>-7.193035369557796</t>
+  </si>
+  <si>
+    <t>-4.964945230582462</t>
+  </si>
+  <si>
+    <t>46.50053412110406</t>
   </si>
   <si>
     <t>0.39428273522074164</t>
@@ -295,28 +295,28 @@
     <t>11.52428125156565</t>
   </si>
   <si>
-    <t>-63.420982772657304</t>
-  </si>
-  <si>
-    <t>45.02398789092384</t>
-  </si>
-  <si>
-    <t>-42.0476104834624</t>
-  </si>
-  <si>
-    <t>32.26109567806575</t>
+    <t>-63.478621269151944</t>
+  </si>
+  <si>
+    <t>44.63637025208568</t>
+  </si>
+  <si>
+    <t>-42.2805951358408</t>
+  </si>
+  <si>
+    <t>32.350704674675875</t>
   </si>
   <si>
     <t>sub_leaf_6</t>
   </si>
   <si>
-    <t>-35.69223966761786</t>
-  </si>
-  <si>
-    <t>-64.12503882579095</t>
-  </si>
-  <si>
-    <t>50.72933203675473</t>
+    <t>-35.657918805343776</t>
+  </si>
+  <si>
+    <t>-64.12503882579094</t>
+  </si>
+  <si>
+    <t>50.77754265668545</t>
   </si>
   <si>
     <t>154.59292641032692</t>
@@ -343,19 +343,19 @@
     <t>-78.5186279093085</t>
   </si>
   <si>
-    <t>35.56694773224588</t>
+    <t>35.669910319068116</t>
   </si>
   <si>
     <t>sub_leaf_7</t>
   </si>
   <si>
-    <t>6.070738168030725</t>
-  </si>
-  <si>
-    <t>39.363418170605705</t>
-  </si>
-  <si>
-    <t>44.02958802570318</t>
+    <t>6.1227293717111895</t>
+  </si>
+  <si>
+    <t>39.48392088041287</t>
+  </si>
+  <si>
+    <t>43.986563962723174</t>
   </si>
   <si>
     <t>0.0724181127538227</t>
@@ -379,28 +379,28 @@
     <t>5</t>
   </si>
   <si>
-    <t>-50.014966639368545</t>
-  </si>
-  <si>
-    <t>-45.554068369370086</t>
-  </si>
-  <si>
-    <t>44.842795260311505</t>
-  </si>
-  <si>
-    <t>41.71651241797505</t>
+    <t>-49.986510396819845</t>
+  </si>
+  <si>
+    <t>-45.37203067897739</t>
+  </si>
+  <si>
+    <t>44.85123563274374</t>
+  </si>
+  <si>
+    <t>41.637031421196575</t>
   </si>
   <si>
     <t>sub_leaf_8</t>
   </si>
   <si>
-    <t>-13.351267345975979</t>
-  </si>
-  <si>
-    <t>-12.371830583187212</t>
-  </si>
-  <si>
-    <t>48.1214049460452</t>
+    <t>-13.420640582687634</t>
+  </si>
+  <si>
+    <t>-12.370673454746896</t>
+  </si>
+  <si>
+    <t>48.18750805764982</t>
   </si>
   <si>
     <t>0.28126467975090946</t>
@@ -424,34 +424,34 @@
     <t>6</t>
   </si>
   <si>
-    <t>30.720433098962136</t>
-  </si>
-  <si>
-    <t>-71.62470029295248</t>
-  </si>
-  <si>
-    <t>-52.75348378699806</t>
-  </si>
-  <si>
-    <t>28.009822620623638</t>
-  </si>
-  <si>
-    <t>-58.306700010311275</t>
-  </si>
-  <si>
-    <t>43.84702429482017</t>
+    <t>30.72159022740245</t>
+  </si>
+  <si>
+    <t>-71.62354316451218</t>
+  </si>
+  <si>
+    <t>-52.75232665855775</t>
+  </si>
+  <si>
+    <t>28.010979749063956</t>
+  </si>
+  <si>
+    <t>-58.72872507278277</t>
+  </si>
+  <si>
+    <t>43.848181423260485</t>
   </si>
   <si>
     <t>sub_leaf_9</t>
   </si>
   <si>
-    <t>-24.21582632878154</t>
-  </si>
-  <si>
-    <t>-47.6048969763473</t>
-  </si>
-  <si>
-    <t>51.567206126551696</t>
+    <t>-24.298569096677017</t>
+  </si>
+  <si>
+    <t>-47.560640312697444</t>
+  </si>
+  <si>
+    <t>51.51886498524703</t>
   </si>
   <si>
     <t>0.7133938885508732</t>
@@ -472,28 +472,28 @@
     <t>149.0391599568673</t>
   </si>
   <si>
-    <t>-92.16758154716233</t>
-  </si>
-  <si>
-    <t>-53.43252148827322</t>
-  </si>
-  <si>
-    <t>38.378194594089344</t>
-  </si>
-  <si>
-    <t>33.74767377378584</t>
+    <t>-92.16107565953361</t>
+  </si>
+  <si>
+    <t>-53.60667365291955</t>
+  </si>
+  <si>
+    <t>38.5199838889373</t>
+  </si>
+  <si>
+    <t>33.31556025282822</t>
   </si>
   <si>
     <t>sub_leaf_10</t>
   </si>
   <si>
-    <t>0.5436438980255804</t>
-  </si>
-  <si>
-    <t>1.1107880255880183</t>
-  </si>
-  <si>
-    <t>39.31185151147227</t>
+    <t>0.5603904517009131</t>
+  </si>
+  <si>
+    <t>1.2049145288685565</t>
+  </si>
+  <si>
+    <t>39.43792487562386</t>
   </si>
   <si>
     <t>12.923498989878858</t>
@@ -514,16 +514,16 @@
     <t>16.76451972611114</t>
   </si>
   <si>
-    <t>-41.49590915749956</t>
-  </si>
-  <si>
-    <t>38.12753195734236</t>
-  </si>
-  <si>
-    <t>41.448908698425846</t>
-  </si>
-  <si>
-    <t>-35.90595590616633</t>
+    <t>-41.67196532688721</t>
+  </si>
+  <si>
+    <t>38.35758965183823</t>
+  </si>
+  <si>
+    <t>41.50369807595375</t>
+  </si>
+  <si>
+    <t>-35.94776059410112</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
avoid overlapping on showing numbers of sub veins in vein_bgr.jpg
</commit_message>
<xml_diff>
--- a/vein_data/vein_general.xlsx
+++ b/vein_data/vein_general.xlsx
@@ -97,13 +97,13 @@
     <t>sub_leaf_1</t>
   </si>
   <si>
-    <t>-6.782253339837299</t>
-  </si>
-  <si>
-    <t>-0.20456564967241775</t>
-  </si>
-  <si>
-    <t>53.10851737952483</t>
+    <t>-6.6559480162360725</t>
+  </si>
+  <si>
+    <t>0.05868961271903217</t>
+  </si>
+  <si>
+    <t>53.01895184036078</t>
   </si>
   <si>
     <t>27.41348121881259</t>
@@ -127,28 +127,28 @@
     <t>4</t>
   </si>
   <si>
-    <t>-75.27386634281146</t>
-  </si>
-  <si>
-    <t>-41.69146886217747</t>
-  </si>
-  <si>
-    <t>41.28233756283264</t>
-  </si>
-  <si>
-    <t>48.5539842828071</t>
+    <t>-75.28451095800045</t>
+  </si>
+  <si>
+    <t>-41.154313722205565</t>
+  </si>
+  <si>
+    <t>41.27169294764363</t>
+  </si>
+  <si>
+    <t>48.54333966761809</t>
   </si>
   <si>
     <t>sub_leaf_2</t>
   </si>
   <si>
-    <t>-0.30890568620245773</t>
-  </si>
-  <si>
-    <t>1.34241802464701</t>
-  </si>
-  <si>
-    <t>42.580041408615855</t>
+    <t>-0.19837811831062346</t>
+  </si>
+  <si>
+    <t>1.4192536029363474</t>
+  </si>
+  <si>
+    <t>42.68215859751152</t>
   </si>
   <si>
     <t>0.1650105616827134</t>
@@ -169,28 +169,28 @@
     <t>0.38962323077198296</t>
   </si>
   <si>
-    <t>-46.288270262894805</t>
-  </si>
-  <si>
-    <t>42.03259995738133</t>
-  </si>
-  <si>
-    <t>42.367811468790954</t>
-  </si>
-  <si>
-    <t>-39.34776390808731</t>
+    <t>-46.27987070385327</t>
+  </si>
+  <si>
+    <t>42.17787155491847</t>
+  </si>
+  <si>
+    <t>42.64785102473808</t>
+  </si>
+  <si>
+    <t>-39.33936434904577</t>
   </si>
   <si>
     <t>sub_leaf_3</t>
   </si>
   <si>
-    <t>33.92211654331513</t>
-  </si>
-  <si>
-    <t>51.48826472585644</t>
-  </si>
-  <si>
-    <t>44.875099521691986</t>
+    <t>33.8602244806344</t>
+  </si>
+  <si>
+    <t>51.395636417917046</t>
+  </si>
+  <si>
+    <t>44.866183537550796</t>
   </si>
   <si>
     <t>0.15044135295302438</t>
@@ -211,28 +211,28 @@
     <t>163.26074768674525</t>
   </si>
   <si>
-    <t>74.2387529794948</t>
-  </si>
-  <si>
-    <t>-41.52681625794717</t>
-  </si>
-  <si>
-    <t>59.233794727365634</t>
-  </si>
-  <si>
-    <t>43.74273472434724</t>
+    <t>74.22259317996169</t>
+  </si>
+  <si>
+    <t>-41.57296809325818</t>
+  </si>
+  <si>
+    <t>59.064697911019955</t>
+  </si>
+  <si>
+    <t>43.72657492481414</t>
   </si>
   <si>
     <t>sub_leaf_4</t>
   </si>
   <si>
-    <t>21.996248083321447</t>
-  </si>
-  <si>
-    <t>46.805060137145375</t>
-  </si>
-  <si>
-    <t>48.1850912717703</t>
+    <t>21.993469305584206</t>
+  </si>
+  <si>
+    <t>46.80857627733623</t>
+  </si>
+  <si>
+    <t>48.17201427980745</t>
   </si>
   <si>
     <t>2.85908802149332</t>
@@ -253,28 +253,28 @@
     <t>38.81331819256618</t>
   </si>
   <si>
-    <t>55.59021296997648</t>
-  </si>
-  <si>
-    <t>-61.215340910981425</t>
-  </si>
-  <si>
-    <t>45.47563306716019</t>
-  </si>
-  <si>
-    <t>48.134487207130555</t>
+    <t>55.55192158709969</t>
+  </si>
+  <si>
+    <t>-61.19519691943532</t>
+  </si>
+  <si>
+    <t>45.38224124859202</t>
+  </si>
+  <si>
+    <t>48.234911306080434</t>
   </si>
   <si>
     <t>sub_leaf_5</t>
   </si>
   <si>
-    <t>-7.193035369557796</t>
-  </si>
-  <si>
-    <t>-4.964945230582462</t>
-  </si>
-  <si>
-    <t>46.50053412110406</t>
+    <t>-7.128249775739491</t>
+  </si>
+  <si>
+    <t>-5.019466295626227</t>
+  </si>
+  <si>
+    <t>46.58977291779643</t>
   </si>
   <si>
     <t>0.39428273522074164</t>
@@ -295,28 +295,28 @@
     <t>11.52428125156565</t>
   </si>
   <si>
-    <t>-63.478621269151944</t>
-  </si>
-  <si>
-    <t>44.63637025208568</t>
-  </si>
-  <si>
-    <t>-42.2805951358408</t>
-  </si>
-  <si>
-    <t>32.350704674675875</t>
+    <t>-63.48833772415064</t>
+  </si>
+  <si>
+    <t>45.01427121244513</t>
+  </si>
+  <si>
+    <t>-42.290311590839494</t>
+  </si>
+  <si>
+    <t>32.25137899958704</t>
   </si>
   <si>
     <t>sub_leaf_6</t>
   </si>
   <si>
-    <t>-35.657918805343776</t>
-  </si>
-  <si>
-    <t>-64.12503882579094</t>
-  </si>
-  <si>
-    <t>50.77754265668545</t>
+    <t>-35.72793970228871</t>
+  </si>
+  <si>
+    <t>-64.3733722638362</t>
+  </si>
+  <si>
+    <t>50.78910541833564</t>
   </si>
   <si>
     <t>154.59292641032692</t>
@@ -340,22 +340,22 @@
     <t>3</t>
   </si>
   <si>
-    <t>-78.5186279093085</t>
-  </si>
-  <si>
-    <t>35.669910319068116</t>
+    <t>-78.44800770501213</t>
+  </si>
+  <si>
+    <t>35.63756086198221</t>
   </si>
   <si>
     <t>sub_leaf_7</t>
   </si>
   <si>
-    <t>6.1227293717111895</t>
-  </si>
-  <si>
-    <t>39.48392088041287</t>
-  </si>
-  <si>
-    <t>43.986563962723174</t>
+    <t>6.099285711554951</t>
+  </si>
+  <si>
+    <t>39.49336304668445</t>
+  </si>
+  <si>
+    <t>44.031188642542645</t>
   </si>
   <si>
     <t>0.0724181127538227</t>
@@ -379,28 +379,28 @@
     <t>5</t>
   </si>
   <si>
-    <t>-49.986510396819845</t>
-  </si>
-  <si>
-    <t>-45.37203067897739</t>
-  </si>
-  <si>
-    <t>44.85123563274374</t>
-  </si>
-  <si>
-    <t>41.637031421196575</t>
+    <t>-49.97706823054826</t>
+  </si>
+  <si>
+    <t>-45.544626203098446</t>
+  </si>
+  <si>
+    <t>44.79880536049031</t>
+  </si>
+  <si>
+    <t>41.72595458424669</t>
   </si>
   <si>
     <t>sub_leaf_8</t>
   </si>
   <si>
-    <t>-13.420640582687634</t>
-  </si>
-  <si>
-    <t>-12.370673454746896</t>
-  </si>
-  <si>
-    <t>48.18750805764982</t>
+    <t>-13.297306885160703</t>
+  </si>
+  <si>
+    <t>-12.320497346273104</t>
+  </si>
+  <si>
+    <t>47.91974240997002</t>
   </si>
   <si>
     <t>0.28126467975090946</t>
@@ -424,34 +424,34 @@
     <t>6</t>
   </si>
   <si>
-    <t>30.72159022740245</t>
-  </si>
-  <si>
-    <t>-71.62354316451218</t>
-  </si>
-  <si>
-    <t>-52.75232665855775</t>
-  </si>
-  <si>
-    <t>28.010979749063956</t>
-  </si>
-  <si>
-    <t>-58.72872507278277</t>
-  </si>
-  <si>
-    <t>43.848181423260485</t>
+    <t>30.727605220104557</t>
+  </si>
+  <si>
+    <t>-71.04716843815358</t>
+  </si>
+  <si>
+    <t>-52.65798943431227</t>
+  </si>
+  <si>
+    <t>28.016994741766062</t>
+  </si>
+  <si>
+    <t>-58.29952788916886</t>
+  </si>
+  <si>
+    <t>43.47624448879986</t>
   </si>
   <si>
     <t>sub_leaf_9</t>
   </si>
   <si>
-    <t>-24.298569096677017</t>
-  </si>
-  <si>
-    <t>-47.560640312697444</t>
-  </si>
-  <si>
-    <t>51.51886498524703</t>
+    <t>-24.366290878913635</t>
+  </si>
+  <si>
+    <t>-47.136113688328564</t>
+  </si>
+  <si>
+    <t>51.603847160216574</t>
   </si>
   <si>
     <t>0.7133938885508732</t>
@@ -472,28 +472,28 @@
     <t>149.0391599568673</t>
   </si>
   <si>
-    <t>-92.16107565953361</t>
+    <t>-92.76822839730893</t>
   </si>
   <si>
     <t>-53.60667365291955</t>
   </si>
   <si>
-    <t>38.5199838889373</t>
-  </si>
-  <si>
-    <t>33.31556025282822</t>
+    <t>38.38470048171806</t>
+  </si>
+  <si>
+    <t>33.29486086227083</t>
   </si>
   <si>
     <t>sub_leaf_10</t>
   </si>
   <si>
-    <t>0.5603904517009131</t>
-  </si>
-  <si>
-    <t>1.2049145288685565</t>
-  </si>
-  <si>
-    <t>39.43792487562386</t>
+    <t>0.601355136578384</t>
+  </si>
+  <si>
+    <t>1.1107878774119335</t>
+  </si>
+  <si>
+    <t>39.37198318836386</t>
   </si>
   <si>
     <t>12.923498989878858</t>
@@ -514,16 +514,16 @@
     <t>16.76451972611114</t>
   </si>
   <si>
-    <t>-41.67196532688721</t>
-  </si>
-  <si>
-    <t>38.35758965183823</t>
-  </si>
-  <si>
-    <t>41.50369807595375</t>
-  </si>
-  <si>
-    <t>-35.94776059410112</t>
+    <t>-41.495909305675646</t>
+  </si>
+  <si>
+    <t>38.12753180916628</t>
+  </si>
+  <si>
+    <t>41.679754097165315</t>
+  </si>
+  <si>
+    <t>-35.90595605434241</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Use lighter color for labelling
</commit_message>
<xml_diff>
--- a/vein_data/vein_general.xlsx
+++ b/vein_data/vein_general.xlsx
@@ -97,13 +97,13 @@
     <t>sub_leaf_1</t>
   </si>
   <si>
-    <t>-6.774989806491423</t>
-  </si>
-  <si>
-    <t>-0.009953478197441967</t>
-  </si>
-  <si>
-    <t>52.95322072716004</t>
+    <t>-6.7811680951745945</t>
+  </si>
+  <si>
+    <t>-0.18797690491407337</t>
+  </si>
+  <si>
+    <t>53.098332452860106</t>
   </si>
   <si>
     <t>27.41348121881259</t>
@@ -127,28 +127,28 @@
     <t>4</t>
   </si>
   <si>
-    <t>-75.28451095800045</t>
-  </si>
-  <si>
-    <t>-41.2915999040385</t>
-  </si>
-  <si>
-    <t>41.271692947643615</t>
-  </si>
-  <si>
-    <t>48.20445868842964</t>
+    <t>-75.28828459824439</t>
+  </si>
+  <si>
+    <t>-41.64387311722784</t>
+  </si>
+  <si>
+    <t>41.267919307399694</t>
+  </si>
+  <si>
+    <t>48.53956602737416</t>
   </si>
   <si>
     <t>sub_leaf_2</t>
   </si>
   <si>
-    <t>-0.2468905793846332</t>
-  </si>
-  <si>
-    <t>1.0978467476340512</t>
-  </si>
-  <si>
-    <t>42.40310115748908</t>
+    <t>-0.3602560427839556</t>
+  </si>
+  <si>
+    <t>1.0978467476340938</t>
+  </si>
+  <si>
+    <t>42.505066876072696</t>
   </si>
   <si>
     <t>0.1650105616827134</t>
@@ -169,28 +169,28 @@
     <t>0.38962323077198296</t>
   </si>
   <si>
-    <t>-45.84809981305198</t>
-  </si>
-  <si>
-    <t>41.51806486880661</t>
-  </si>
-  <si>
-    <t>42.664844000245346</t>
-  </si>
-  <si>
-    <t>-39.32237137353851</t>
+    <t>-46.26287772834596</t>
+  </si>
+  <si>
+    <t>41.518064868806654</t>
+  </si>
+  <si>
+    <t>42.62616006194195</t>
+  </si>
+  <si>
+    <t>-39.322371373538466</t>
   </si>
   <si>
     <t>sub_leaf_3</t>
   </si>
   <si>
-    <t>33.87630161470989</t>
-  </si>
-  <si>
-    <t>51.411796417924975</t>
-  </si>
-  <si>
-    <t>44.86632285946189</t>
+    <t>33.59474241236954</t>
+  </si>
+  <si>
+    <t>51.3791413042813</t>
+  </si>
+  <si>
+    <t>44.697679144728774</t>
   </si>
   <si>
     <t>0.15044135295302438</t>
@@ -211,28 +211,28 @@
     <t>163.26074768674525</t>
   </si>
   <si>
-    <t>74.2387531799696</t>
-  </si>
-  <si>
-    <t>-41.55713955697999</t>
-  </si>
-  <si>
-    <t>59.080857911027884</t>
-  </si>
-  <si>
-    <t>43.74273492482207</t>
+    <t>73.28907794449847</t>
+  </si>
+  <si>
+    <t>-41.66839090358291</t>
+  </si>
+  <si>
+    <t>59.085660814902106</t>
+  </si>
+  <si>
+    <t>43.67262179366049</t>
   </si>
   <si>
     <t>sub_leaf_4</t>
   </si>
   <si>
-    <t>21.911164003292406</t>
-  </si>
-  <si>
-    <t>46.63788847083477</t>
-  </si>
-  <si>
-    <t>48.14075182281277</t>
+    <t>22.054481794032124</t>
+  </si>
+  <si>
+    <t>46.78843228579012</t>
+  </si>
+  <si>
+    <t>48.1090131792516</t>
   </si>
   <si>
     <t>2.85908802149332</t>
@@ -253,28 +253,28 @@
     <t>38.81331819256618</t>
   </si>
   <si>
-    <t>55.587216476229</t>
-  </si>
-  <si>
-    <t>-61.2183374047289</t>
-  </si>
-  <si>
-    <t>45.472636573412714</t>
-  </si>
-  <si>
-    <t>47.80314036825681</t>
+    <t>55.65905418973773</t>
+  </si>
+  <si>
+    <t>-61.01799158518947</t>
+  </si>
+  <si>
+    <t>45.36209725704591</t>
+  </si>
+  <si>
+    <t>48.21476731453433</t>
   </si>
   <si>
     <t>sub_leaf_5</t>
   </si>
   <si>
-    <t>-7.34335859467894</t>
-  </si>
-  <si>
-    <t>-5.265591904304765</t>
-  </si>
-  <si>
-    <t>46.37325481586868</t>
+    <t>-7.206270743291331</t>
+  </si>
+  <si>
+    <t>-5.009749617147527</t>
+  </si>
+  <si>
+    <t>46.69603663169677</t>
   </si>
   <si>
     <t>0.39428273522074164</t>
@@ -295,28 +295,28 @@
     <t>11.52428125156565</t>
   </si>
   <si>
-    <t>-63.47862104567193</t>
-  </si>
-  <si>
-    <t>44.6363704755657</t>
-  </si>
-  <si>
-    <t>-42.28059491236078</t>
-  </si>
-  <si>
-    <t>31.749411103751253</t>
+    <t>-63.8295716297941</t>
+  </si>
+  <si>
+    <t>45.023987890923834</t>
+  </si>
+  <si>
+    <t>-42.2805949123608</t>
+  </si>
+  <si>
+    <t>32.26109567806574</t>
   </si>
   <si>
     <t>sub_leaf_6</t>
   </si>
   <si>
-    <t>-35.716424695781065</t>
-  </si>
-  <si>
-    <t>-64.11895990268108</t>
-  </si>
-  <si>
-    <t>50.825211066019804</t>
+    <t>-35.65015784612282</t>
+  </si>
+  <si>
+    <t>-64.11421157479182</t>
+  </si>
+  <si>
+    <t>50.77323540196945</t>
   </si>
   <si>
     <t>154.59292641032692</t>
@@ -340,22 +340,22 @@
     <t>3</t>
   </si>
   <si>
-    <t>-78.69710455150559</t>
-  </si>
-  <si>
-    <t>35.666790366843486</t>
+    <t>-78.50780065830939</t>
+  </si>
+  <si>
+    <t>35.671538694732746</t>
   </si>
   <si>
     <t>sub_leaf_7</t>
   </si>
   <si>
-    <t>6.162347597545848</t>
-  </si>
-  <si>
-    <t>39.363418170605705</t>
-  </si>
-  <si>
-    <t>43.93457244485874</t>
+    <t>6.131246248070719</t>
+  </si>
+  <si>
+    <t>39.48392088041285</t>
+  </si>
+  <si>
+    <t>44.00518345892174</t>
   </si>
   <si>
     <t>0.0724181127538227</t>
@@ -379,28 +379,28 @@
     <t>5</t>
   </si>
   <si>
-    <t>-49.994358853172656</t>
-  </si>
-  <si>
-    <t>-45.147395715627326</t>
-  </si>
-  <si>
-    <t>44.87356196794846</t>
-  </si>
-  <si>
-    <t>41.71651241797505</t>
+    <t>-50.0149666393685</t>
+  </si>
+  <si>
+    <t>-45.3720306789774</t>
+  </si>
+  <si>
+    <t>44.84279526031155</t>
+  </si>
+  <si>
+    <t>41.716512417975096</t>
   </si>
   <si>
     <t>sub_leaf_8</t>
   </si>
   <si>
-    <t>-13.337896433266037</t>
-  </si>
-  <si>
-    <t>-12.294618935857592</t>
-  </si>
-  <si>
-    <t>48.23315689169455</t>
+    <t>-13.341634463113877</t>
+  </si>
+  <si>
+    <t>-12.245968813072313</t>
+  </si>
+  <si>
+    <t>47.96643435536334</t>
   </si>
   <si>
     <t>0.28126467975090946</t>
@@ -424,34 +424,34 @@
     <t>6</t>
   </si>
   <si>
-    <t>30.725443202707034</t>
-  </si>
-  <si>
-    <t>-71.61969018920759</t>
-  </si>
-  <si>
-    <t>-52.60407059608372</t>
-  </si>
-  <si>
-    <t>28.01483272436854</t>
-  </si>
-  <si>
-    <t>-58.72487209747819</t>
-  </si>
-  <si>
-    <t>44.180978356097725</t>
+    <t>30.729645134302352</t>
+  </si>
+  <si>
+    <t>-71.04512852395577</t>
+  </si>
+  <si>
+    <t>-52.51097228210848</t>
+  </si>
+  <si>
+    <t>28.019034655963857</t>
+  </si>
+  <si>
+    <t>-58.72067016588287</t>
+  </si>
+  <si>
+    <t>43.47828440299765</t>
   </si>
   <si>
     <t>sub_leaf_9</t>
   </si>
   <si>
-    <t>-24.41285630675775</t>
-  </si>
-  <si>
-    <t>-47.59839108871858</t>
-  </si>
-  <si>
-    <t>51.56592324389232</t>
+    <t>-24.193722390095967</t>
+  </si>
+  <si>
+    <t>-47.604896876944316</t>
+  </si>
+  <si>
+    <t>51.45740053082853</t>
   </si>
   <si>
     <t>0.7133938885508732</t>
@@ -472,28 +472,28 @@
     <t>149.0391599568673</t>
   </si>
   <si>
-    <t>-92.36998137650835</t>
-  </si>
-  <si>
-    <t>-53.79616980310808</t>
-  </si>
-  <si>
-    <t>38.38470048171806</t>
-  </si>
-  <si>
-    <t>33.31556025282822</t>
+    <t>-92.16758144775933</t>
+  </si>
+  <si>
+    <t>-53.03325700797723</t>
+  </si>
+  <si>
+    <t>38.378194693492325</t>
+  </si>
+  <si>
+    <t>33.45892868870871</t>
   </si>
   <si>
     <t>sub_leaf_10</t>
   </si>
   <si>
-    <t>0.6578660450860028</t>
-  </si>
-  <si>
-    <t>1.3809706982562062</t>
-  </si>
-  <si>
-    <t>39.33895579173429</t>
+    <t>0.6338835804533058</t>
+  </si>
+  <si>
+    <t>1.100474317491166</t>
+  </si>
+  <si>
+    <t>39.32581387373229</t>
   </si>
   <si>
     <t>12.923498989878858</t>
@@ -517,10 +517,10 @@
     <t>-41.46257977990643</t>
   </si>
   <si>
-    <t>38.53364582122588</t>
-  </si>
-  <si>
-    <t>41.332102563738026</t>
+    <t>37.9726530596958</t>
+  </si>
+  <si>
+    <t>41.79716546673732</t>
   </si>
   <si>
     <t>-35.77170442471347</t>

</xml_diff>